<commit_message>
Added a selected minimisation file to master results file
</commit_message>
<xml_diff>
--- a/Master_Results_File.xlsx
+++ b/Master_Results_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ct6g18/Python/org-alk-sausage-machine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5971379-8AD0-4940-A7B8-BF8649B75A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1F5EFF-C680-A543-B1F8-313431D80767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="48220" yWindow="14760" windowWidth="20380" windowHeight="13860" xr2:uid="{A99928C4-377B-FA4A-8AFD-F264DD9F788A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>MASS</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>SSR</t>
+  </si>
+  <si>
+    <t>SELECTED_MINIMISATION</t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,7 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,7 +460,7 @@
     <col min="17" max="20" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -508,6 +511,9 @@
       </c>
       <c r="Q1" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>